<commit_message>
All current tests now pass
Mostly work in arcs and the parent classes of arc.
</commit_message>
<xml_diff>
--- a/NVcad/CadObjects/documentation_partial/Arcs.xlsx
+++ b/NVcad/CadObjects/documentation_partial/Arcs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="42">
   <si>
     <t>Constructor Description</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Is computed on the fly?</t>
   </si>
   <si>
-    <t>Could never be in constructor?</t>
-  </si>
-  <si>
     <t>Bounding Box</t>
   </si>
   <si>
@@ -130,6 +127,21 @@
   </si>
   <si>
     <t>Source class</t>
+  </si>
+  <si>
+    <t>Arc_CreateArc_ctor3DeflectingLeft90_IsCorrect</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Arc_CreateArc_ctor3DeflectingRight90_IsCorrect</t>
+  </si>
+  <si>
+    <t>May be in constructor</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -487,27 +499,27 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="61.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="93.6" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>
@@ -522,28 +534,28 @@
         <v>5</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="N2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -565,217 +577,289 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="O8" t="s">
         <v>19</v>
       </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>20</v>
-      </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
@@ -784,6 +868,22 @@
       </c>
       <c r="B11" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="11:11" x14ac:dyDescent="0.3">

</xml_diff>